<commit_message>
write the times in separate excel sheet
</commit_message>
<xml_diff>
--- a/data/amiris/amiris_data_structure.xlsx
+++ b/data/amiris/amiris_data_structure.xlsx
@@ -13,6 +13,7 @@
     <sheet name="renewables" sheetId="5" state="visible" r:id="rId5"/>
     <sheet name="storages" sheetId="6" state="visible" r:id="rId6"/>
     <sheet name="scenario_data_emlab" sheetId="7" state="visible" r:id="rId7"/>
+    <sheet name="times" sheetId="8" state="visible" r:id="rId8"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="191029" fullCalcOnLoad="1"/>
@@ -21,7 +22,10 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="0"/>
+  <numFmts count="2">
+    <numFmt numFmtId="164" formatCode="yyyy-mm-dd h:mm:ss"/>
+    <numFmt numFmtId="165" formatCode="YYYY-MM-DD HH:MM:SS"/>
+  </numFmts>
   <fonts count="4">
     <font>
       <name val="Calibri"/>
@@ -81,7 +85,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
@@ -89,6 +93,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="top"/>
     </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -12430,7 +12435,7 @@
       </c>
       <c r="C1" s="4" t="inlineStr">
         <is>
-          <t>Storage</t>
+          <t>StorageType</t>
         </is>
       </c>
       <c r="D1" s="4" t="inlineStr">
@@ -12526,7 +12531,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C10"/>
+  <dimension ref="A1:C8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -12545,130 +12550,140 @@
     <row r="2">
       <c r="A2" s="4" t="inlineStr">
         <is>
-          <t>StartTime</t>
-        </is>
-      </c>
-      <c r="B2" t="inlineStr">
-        <is>
-          <t>['01-01-2025']</t>
-        </is>
-      </c>
-      <c r="C2" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> </t>
-        </is>
+          <t>Co2Prices</t>
+        </is>
+      </c>
+      <c r="B2" t="n">
+        <v>36.31999999999999</v>
+      </c>
+      <c r="C2" t="n">
+        <v>40.3</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="4" t="inlineStr">
         <is>
-          <t>StopTime</t>
-        </is>
-      </c>
-      <c r="B3" t="inlineStr">
-        <is>
-          <t>['31-12-2025']</t>
-        </is>
-      </c>
-      <c r="C3" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> </t>
-        </is>
+          <t>FuelPrice_NUCLEAR</t>
+        </is>
+      </c>
+      <c r="B3" t="n">
+        <v>1.69</v>
+      </c>
+      <c r="C3" t="n">
+        <v>1.69</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="4" t="inlineStr">
         <is>
-          <t>Co2Prices</t>
+          <t>FuelPrice_LIGNITE</t>
         </is>
       </c>
       <c r="B4" t="n">
-        <v>36.31999999999999</v>
+        <v>3.96</v>
       </c>
       <c r="C4" t="n">
-        <v>40.3</v>
+        <v>3.96</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="4" t="inlineStr">
         <is>
-          <t>FuelPrice_NUCLEAR</t>
+          <t>FuelPrice_HARD_COAL</t>
         </is>
       </c>
       <c r="B5" t="n">
-        <v>1.69</v>
+        <v>13.616</v>
       </c>
       <c r="C5" t="n">
-        <v>1.69</v>
+        <v>14.32</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="4" t="inlineStr">
         <is>
-          <t>FuelPrice_LIGNITE</t>
+          <t>FuelPrice_NATURAL_GAS</t>
         </is>
       </c>
       <c r="B6" t="n">
-        <v>3.96</v>
+        <v>21.392</v>
       </c>
       <c r="C6" t="n">
-        <v>3.96</v>
+        <v>21.7</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="4" t="inlineStr">
         <is>
-          <t>FuelPrice_HARD_COAL</t>
+          <t>FuelPrice_OIL</t>
         </is>
       </c>
       <c r="B7" t="n">
-        <v>13.616</v>
+        <v>53.136</v>
       </c>
       <c r="C7" t="n">
-        <v>14.32</v>
+        <v>54.81</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="4" t="inlineStr">
         <is>
-          <t>FuelPrice_NATURAL_GAS</t>
-        </is>
-      </c>
-      <c r="B8" t="n">
-        <v>21.392</v>
-      </c>
-      <c r="C8" t="n">
-        <v>21.7</v>
-      </c>
-    </row>
-    <row r="9">
-      <c r="A9" s="4" t="inlineStr">
-        <is>
-          <t>FuelPrice_OIL</t>
-        </is>
-      </c>
-      <c r="B9" t="n">
-        <v>53.136</v>
-      </c>
-      <c r="C9" t="n">
-        <v>54.81</v>
-      </c>
-    </row>
-    <row r="10">
-      <c r="A10" s="4" t="inlineStr">
-        <is>
           <t>DemandSeries</t>
         </is>
       </c>
-      <c r="B10" t="inlineStr">
+      <c r="B8" t="inlineStr">
         <is>
           <t>./timeseries/demand/load.csv</t>
         </is>
       </c>
-      <c r="C10" t="inlineStr">
+      <c r="C8" t="inlineStr">
         <is>
           <t>./timeseries/demand/load.csv</t>
         </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:B3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="B1" s="4" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="4" t="inlineStr">
+        <is>
+          <t>StartTime</t>
+        </is>
+      </c>
+      <c r="B2" s="5" t="n">
+        <v>45657.99861111111</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="4" t="inlineStr">
+        <is>
+          <t>StopTime</t>
+        </is>
+      </c>
+      <c r="B3" s="5" t="n">
+        <v>46021.99861111111</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
moved from open amiris yamls debug
</commit_message>
<xml_diff>
--- a/data/amiris/amiris_data_structure.xlsx
+++ b/data/amiris/amiris_data_structure.xlsx
@@ -25,8 +25,8 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="3">
     <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd\ hh:mm:ss"/>
-    <numFmt numFmtId="165" formatCode="yyyy-mm-dd h:mm:ss"/>
-    <numFmt numFmtId="166" formatCode="YYYY-MM-DD HH:MM:SS"/>
+    <numFmt numFmtId="165" formatCode="YYYY-MM-DD HH:MM:SS"/>
+    <numFmt numFmtId="166" formatCode="yyyy-mm-dd h:mm:ss"/>
   </numFmts>
   <fonts count="5">
     <font>
@@ -107,7 +107,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
@@ -119,7 +119,8 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="2" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -1165,7 +1166,7 @@
         <v>0</v>
       </c>
       <c r="B2" t="n">
-        <v>0</v>
+        <v>20151700021</v>
       </c>
       <c r="C2" t="inlineStr">
         <is>
@@ -1190,7 +1191,7 @@
         <v>1</v>
       </c>
       <c r="B3" t="n">
-        <v>0</v>
+        <v>20013000022</v>
       </c>
       <c r="C3" t="inlineStr">
         <is>
@@ -1215,7 +1216,7 @@
         <v>2</v>
       </c>
       <c r="B4" t="n">
-        <v>0</v>
+        <v>20001700023</v>
       </c>
       <c r="C4" t="inlineStr">
         <is>
@@ -1240,7 +1241,7 @@
         <v>3</v>
       </c>
       <c r="B5" t="n">
-        <v>0</v>
+        <v>19892800024</v>
       </c>
       <c r="C5" t="inlineStr">
         <is>
@@ -1265,7 +1266,7 @@
         <v>4</v>
       </c>
       <c r="B6" t="n">
-        <v>0</v>
+        <v>20140300037</v>
       </c>
       <c r="C6" t="inlineStr">
         <is>
@@ -1290,7 +1291,7 @@
         <v>5</v>
       </c>
       <c r="B7" t="n">
-        <v>0</v>
+        <v>20120300038</v>
       </c>
       <c r="C7" t="inlineStr">
         <is>
@@ -1315,7 +1316,7 @@
         <v>6</v>
       </c>
       <c r="B8" t="n">
-        <v>0</v>
+        <v>20080300039</v>
       </c>
       <c r="C8" t="inlineStr">
         <is>
@@ -1340,7 +1341,7 @@
         <v>7</v>
       </c>
       <c r="B9" t="n">
-        <v>0</v>
+        <v>20060300040</v>
       </c>
       <c r="C9" t="inlineStr">
         <is>
@@ -1365,7 +1366,7 @@
         <v>8</v>
       </c>
       <c r="B10" t="n">
-        <v>0</v>
+        <v>20040300041</v>
       </c>
       <c r="C10" t="inlineStr">
         <is>
@@ -1390,7 +1391,7 @@
         <v>9</v>
       </c>
       <c r="B11" t="n">
-        <v>0</v>
+        <v>20020300042</v>
       </c>
       <c r="C11" t="inlineStr">
         <is>
@@ -1415,7 +1416,7 @@
         <v>10</v>
       </c>
       <c r="B12" t="n">
-        <v>0</v>
+        <v>20000300043</v>
       </c>
       <c r="C12" t="inlineStr">
         <is>
@@ -1440,7 +1441,7 @@
         <v>11</v>
       </c>
       <c r="B13" t="n">
-        <v>0</v>
+        <v>20092800044</v>
       </c>
       <c r="C13" t="inlineStr">
         <is>
@@ -1465,7 +1466,7 @@
         <v>12</v>
       </c>
       <c r="B14" t="n">
-        <v>0</v>
+        <v>20002800045</v>
       </c>
       <c r="C14" t="inlineStr">
         <is>
@@ -1490,7 +1491,7 @@
         <v>13</v>
       </c>
       <c r="B15" t="n">
-        <v>0</v>
+        <v>20033000046</v>
       </c>
       <c r="C15" t="inlineStr">
         <is>
@@ -1515,7 +1516,7 @@
         <v>14</v>
       </c>
       <c r="B16" t="n">
-        <v>0</v>
+        <v>20113000047</v>
       </c>
       <c r="C16" t="inlineStr">
         <is>
@@ -1540,7 +1541,7 @@
         <v>15</v>
       </c>
       <c r="B17" t="n">
-        <v>0</v>
+        <v>20062900048</v>
       </c>
       <c r="C17" t="inlineStr">
         <is>
@@ -1565,7 +1566,7 @@
         <v>16</v>
       </c>
       <c r="B18" t="n">
-        <v>0</v>
+        <v>20032900049</v>
       </c>
       <c r="C18" t="inlineStr">
         <is>
@@ -1590,7 +1591,7 @@
         <v>17</v>
       </c>
       <c r="B19" t="n">
-        <v>20072900051</v>
+        <v>20062900051</v>
       </c>
       <c r="C19" t="inlineStr">
         <is>
@@ -1615,7 +1616,7 @@
         <v>18</v>
       </c>
       <c r="B20" t="n">
-        <v>19882900052</v>
+        <v>19872900052</v>
       </c>
       <c r="C20" t="inlineStr">
         <is>
@@ -1640,7 +1641,7 @@
         <v>19</v>
       </c>
       <c r="B21" t="n">
-        <v>20112900053</v>
+        <v>20102900053</v>
       </c>
       <c r="C21" t="inlineStr">
         <is>
@@ -1665,7 +1666,7 @@
         <v>20</v>
       </c>
       <c r="B22" t="n">
-        <v>19832900054</v>
+        <v>19822900054</v>
       </c>
       <c r="C22" t="inlineStr">
         <is>
@@ -1690,7 +1691,7 @@
         <v>21</v>
       </c>
       <c r="B23" t="n">
-        <v>19892900055</v>
+        <v>19882900055</v>
       </c>
       <c r="C23" t="inlineStr">
         <is>
@@ -1715,7 +1716,7 @@
         <v>22</v>
       </c>
       <c r="B24" t="n">
-        <v>19862900056</v>
+        <v>19852900056</v>
       </c>
       <c r="C24" t="inlineStr">
         <is>
@@ -1740,7 +1741,7 @@
         <v>23</v>
       </c>
       <c r="B25" t="n">
-        <v>19822900058</v>
+        <v>19812900058</v>
       </c>
       <c r="C25" t="inlineStr">
         <is>
@@ -1765,7 +1766,7 @@
         <v>24</v>
       </c>
       <c r="B26" t="n">
-        <v>19881400059</v>
+        <v>19871400059</v>
       </c>
       <c r="C26" t="inlineStr">
         <is>
@@ -1790,7 +1791,7 @@
         <v>25</v>
       </c>
       <c r="B27" t="n">
-        <v>19842900060</v>
+        <v>19832900060</v>
       </c>
       <c r="C27" t="inlineStr">
         <is>
@@ -1815,7 +1816,7 @@
         <v>26</v>
       </c>
       <c r="B28" t="n">
-        <v>20130300061</v>
+        <v>20120300061</v>
       </c>
       <c r="C28" t="inlineStr">
         <is>
@@ -1840,7 +1841,7 @@
         <v>27</v>
       </c>
       <c r="B29" t="n">
-        <v>19981700062</v>
+        <v>19971700062</v>
       </c>
       <c r="C29" t="inlineStr">
         <is>
@@ -1865,7 +1866,7 @@
         <v>28</v>
       </c>
       <c r="B30" t="n">
-        <v>20100300063</v>
+        <v>20090300063</v>
       </c>
       <c r="C30" t="inlineStr">
         <is>
@@ -1890,7 +1891,7 @@
         <v>29</v>
       </c>
       <c r="B31" t="n">
-        <v>20120300065</v>
+        <v>20110300065</v>
       </c>
       <c r="C31" t="inlineStr">
         <is>
@@ -1915,7 +1916,7 @@
         <v>30</v>
       </c>
       <c r="B32" t="n">
-        <v>20153000066</v>
+        <v>20143000066</v>
       </c>
       <c r="C32" t="inlineStr">
         <is>
@@ -1940,7 +1941,7 @@
         <v>31</v>
       </c>
       <c r="B33" t="n">
-        <v>20013000067</v>
+        <v>20003000067</v>
       </c>
       <c r="C33" t="inlineStr">
         <is>
@@ -1965,7 +1966,7 @@
         <v>32</v>
       </c>
       <c r="B34" t="n">
-        <v>19920300068</v>
+        <v>19910300068</v>
       </c>
       <c r="C34" t="inlineStr">
         <is>
@@ -1990,7 +1991,7 @@
         <v>33</v>
       </c>
       <c r="B35" t="n">
-        <v>19950300069</v>
+        <v>19940300069</v>
       </c>
       <c r="C35" t="inlineStr">
         <is>
@@ -2015,7 +2016,7 @@
         <v>34</v>
       </c>
       <c r="B36" t="n">
-        <v>19943000070</v>
+        <v>19933000070</v>
       </c>
       <c r="C36" t="inlineStr">
         <is>
@@ -2040,7 +2041,7 @@
         <v>35</v>
       </c>
       <c r="B37" t="n">
-        <v>19953000071</v>
+        <v>19943000071</v>
       </c>
       <c r="C37" t="inlineStr">
         <is>
@@ -2065,7 +2066,7 @@
         <v>36</v>
       </c>
       <c r="B38" t="n">
-        <v>20163000072</v>
+        <v>20153000072</v>
       </c>
       <c r="C38" t="inlineStr">
         <is>
@@ -2090,7 +2091,7 @@
         <v>37</v>
       </c>
       <c r="B39" t="n">
-        <v>19991700073</v>
+        <v>19981700073</v>
       </c>
       <c r="C39" t="inlineStr">
         <is>
@@ -2115,7 +2116,7 @@
         <v>38</v>
       </c>
       <c r="B40" t="n">
-        <v>20030300074</v>
+        <v>20020300074</v>
       </c>
       <c r="C40" t="inlineStr">
         <is>
@@ -2140,7 +2141,7 @@
         <v>39</v>
       </c>
       <c r="B41" t="n">
-        <v>19941700075</v>
+        <v>19931700075</v>
       </c>
       <c r="C41" t="inlineStr">
         <is>
@@ -2165,7 +2166,7 @@
         <v>40</v>
       </c>
       <c r="B42" t="n">
-        <v>19941700076</v>
+        <v>19931700076</v>
       </c>
       <c r="C42" t="inlineStr">
         <is>
@@ -2190,7 +2191,7 @@
         <v>41</v>
       </c>
       <c r="B43" t="n">
-        <v>19970300077</v>
+        <v>19960300077</v>
       </c>
       <c r="C43" t="inlineStr">
         <is>
@@ -2215,7 +2216,7 @@
         <v>42</v>
       </c>
       <c r="B44" t="n">
-        <v>19950300078</v>
+        <v>19940300078</v>
       </c>
       <c r="C44" t="inlineStr">
         <is>
@@ -2240,7 +2241,7 @@
         <v>43</v>
       </c>
       <c r="B45" t="n">
-        <v>19862800081</v>
+        <v>19852800081</v>
       </c>
       <c r="C45" t="inlineStr">
         <is>
@@ -2265,7 +2266,7 @@
         <v>44</v>
       </c>
       <c r="B46" t="n">
-        <v>20191700082</v>
+        <v>20181700082</v>
       </c>
       <c r="C46" t="inlineStr">
         <is>
@@ -2290,7 +2291,7 @@
         <v>45</v>
       </c>
       <c r="B47" t="n">
-        <v>20021700083</v>
+        <v>20011700083</v>
       </c>
       <c r="C47" t="inlineStr">
         <is>
@@ -2315,7 +2316,7 @@
         <v>46</v>
       </c>
       <c r="B48" t="n">
-        <v>19872900084</v>
+        <v>19862900084</v>
       </c>
       <c r="C48" t="inlineStr">
         <is>
@@ -2340,7 +2341,7 @@
         <v>47</v>
       </c>
       <c r="B49" t="n">
-        <v>19962900085</v>
+        <v>19952900085</v>
       </c>
       <c r="C49" t="inlineStr">
         <is>
@@ -2365,7 +2366,7 @@
         <v>48</v>
       </c>
       <c r="B50" t="n">
-        <v>20082900086</v>
+        <v>20072900086</v>
       </c>
       <c r="C50" t="inlineStr">
         <is>
@@ -2390,7 +2391,7 @@
         <v>49</v>
       </c>
       <c r="B51" t="n">
-        <v>20032800087</v>
+        <v>20022800087</v>
       </c>
       <c r="C51" t="inlineStr">
         <is>
@@ -2415,7 +2416,7 @@
         <v>50</v>
       </c>
       <c r="B52" t="n">
-        <v>20132800088</v>
+        <v>20122800088</v>
       </c>
       <c r="C52" t="inlineStr">
         <is>
@@ -2440,7 +2441,7 @@
         <v>51</v>
       </c>
       <c r="B53" t="n">
-        <v>19892800089</v>
+        <v>19882800089</v>
       </c>
       <c r="C53" t="inlineStr">
         <is>
@@ -2465,7 +2466,7 @@
         <v>52</v>
       </c>
       <c r="B54" t="n">
-        <v>20030300090</v>
+        <v>20020300090</v>
       </c>
       <c r="C54" t="inlineStr">
         <is>
@@ -2490,7 +2491,7 @@
         <v>53</v>
       </c>
       <c r="B55" t="n">
-        <v>19952800091</v>
+        <v>19942800091</v>
       </c>
       <c r="C55" t="inlineStr">
         <is>
@@ -2515,7 +2516,7 @@
         <v>54</v>
       </c>
       <c r="B56" t="n">
-        <v>19922800092</v>
+        <v>19912800092</v>
       </c>
       <c r="C56" t="inlineStr">
         <is>
@@ -2540,7 +2541,7 @@
         <v>55</v>
       </c>
       <c r="B57" t="n">
-        <v>20052800093</v>
+        <v>20042800093</v>
       </c>
       <c r="C57" t="inlineStr">
         <is>
@@ -2565,7 +2566,7 @@
         <v>56</v>
       </c>
       <c r="B58" t="n">
-        <v>20112800094</v>
+        <v>20102800094</v>
       </c>
       <c r="C58" t="inlineStr">
         <is>
@@ -2590,7 +2591,7 @@
         <v>57</v>
       </c>
       <c r="B59" t="n">
-        <v>20133000095</v>
+        <v>20123000095</v>
       </c>
       <c r="C59" t="inlineStr">
         <is>
@@ -2615,7 +2616,7 @@
         <v>58</v>
       </c>
       <c r="B60" t="n">
-        <v>19961700096</v>
+        <v>19951700096</v>
       </c>
       <c r="C60" t="inlineStr">
         <is>
@@ -2640,7 +2641,7 @@
         <v>59</v>
       </c>
       <c r="B61" t="n">
-        <v>20001700097</v>
+        <v>19991700097</v>
       </c>
       <c r="C61" t="inlineStr">
         <is>
@@ -2665,7 +2666,7 @@
         <v>60</v>
       </c>
       <c r="B62" t="n">
-        <v>20060300098</v>
+        <v>20050300098</v>
       </c>
       <c r="C62" t="inlineStr">
         <is>
@@ -2690,7 +2691,7 @@
         <v>61</v>
       </c>
       <c r="B63" t="n">
-        <v>19941700099</v>
+        <v>19931700099</v>
       </c>
       <c r="C63" t="inlineStr">
         <is>
@@ -2715,7 +2716,7 @@
         <v>62</v>
       </c>
       <c r="B64" t="n">
-        <v>19981400101</v>
+        <v>19971400101</v>
       </c>
       <c r="C64" t="inlineStr">
         <is>
@@ -2740,7 +2741,7 @@
         <v>63</v>
       </c>
       <c r="B65" t="n">
-        <v>20050300102</v>
+        <v>20040300102</v>
       </c>
       <c r="C65" t="inlineStr">
         <is>
@@ -2765,7 +2766,7 @@
         <v>64</v>
       </c>
       <c r="B66" t="n">
-        <v>19972800103</v>
+        <v>19962800103</v>
       </c>
       <c r="C66" t="inlineStr">
         <is>
@@ -2790,7 +2791,7 @@
         <v>65</v>
       </c>
       <c r="B67" t="n">
-        <v>19842800104</v>
+        <v>19832800104</v>
       </c>
       <c r="C67" t="inlineStr">
         <is>
@@ -2815,7 +2816,7 @@
         <v>66</v>
       </c>
       <c r="B68" t="n">
-        <v>20161700105</v>
+        <v>20151700105</v>
       </c>
       <c r="C68" t="inlineStr">
         <is>
@@ -2840,7 +2841,7 @@
         <v>67</v>
       </c>
       <c r="B69" t="n">
-        <v>20141700106</v>
+        <v>20131700106</v>
       </c>
       <c r="C69" t="inlineStr">
         <is>
@@ -2865,7 +2866,7 @@
         <v>68</v>
       </c>
       <c r="B70" t="n">
-        <v>19941700107</v>
+        <v>19931700107</v>
       </c>
       <c r="C70" t="inlineStr">
         <is>
@@ -2890,7 +2891,7 @@
         <v>69</v>
       </c>
       <c r="B71" t="n">
-        <v>20051700108</v>
+        <v>20041700108</v>
       </c>
       <c r="C71" t="inlineStr">
         <is>
@@ -2915,7 +2916,7 @@
         <v>70</v>
       </c>
       <c r="B72" t="n">
-        <v>20061700109</v>
+        <v>20051700109</v>
       </c>
       <c r="C72" t="inlineStr">
         <is>
@@ -2940,7 +2941,7 @@
         <v>71</v>
       </c>
       <c r="B73" t="n">
-        <v>19921400111</v>
+        <v>19911400111</v>
       </c>
       <c r="C73" t="inlineStr">
         <is>
@@ -2965,7 +2966,7 @@
         <v>72</v>
       </c>
       <c r="B74" t="n">
-        <v>19960300112</v>
+        <v>19950300112</v>
       </c>
       <c r="C74" t="inlineStr">
         <is>
@@ -2990,7 +2991,7 @@
         <v>73</v>
       </c>
       <c r="B75" t="n">
-        <v>19990300113</v>
+        <v>19980300113</v>
       </c>
       <c r="C75" t="inlineStr">
         <is>
@@ -3015,7 +3016,7 @@
         <v>74</v>
       </c>
       <c r="B76" t="n">
-        <v>20070300114</v>
+        <v>20060300114</v>
       </c>
       <c r="C76" t="inlineStr">
         <is>
@@ -3040,7 +3041,7 @@
         <v>75</v>
       </c>
       <c r="B77" t="n">
-        <v>20060300115</v>
+        <v>20050300115</v>
       </c>
       <c r="C77" t="inlineStr">
         <is>
@@ -3065,7 +3066,7 @@
         <v>76</v>
       </c>
       <c r="B78" t="n">
-        <v>20070300116</v>
+        <v>20060300116</v>
       </c>
       <c r="C78" t="inlineStr">
         <is>
@@ -3090,7 +3091,7 @@
         <v>77</v>
       </c>
       <c r="B79" t="n">
-        <v>20090300117</v>
+        <v>20080300117</v>
       </c>
       <c r="C79" t="inlineStr">
         <is>
@@ -3115,7 +3116,7 @@
         <v>78</v>
       </c>
       <c r="B80" t="n">
-        <v>19930300118</v>
+        <v>19920300118</v>
       </c>
       <c r="C80" t="inlineStr">
         <is>
@@ -3140,7 +3141,7 @@
         <v>79</v>
       </c>
       <c r="B81" t="n">
-        <v>20020300119</v>
+        <v>20010300119</v>
       </c>
       <c r="C81" t="inlineStr">
         <is>
@@ -3165,7 +3166,7 @@
         <v>80</v>
       </c>
       <c r="B82" t="n">
-        <v>20170300120</v>
+        <v>20160300120</v>
       </c>
       <c r="C82" t="inlineStr">
         <is>
@@ -3190,7 +3191,7 @@
         <v>81</v>
       </c>
       <c r="B83" t="n">
-        <v>20060300121</v>
+        <v>20050300121</v>
       </c>
       <c r="C83" t="inlineStr">
         <is>
@@ -3215,7 +3216,7 @@
         <v>82</v>
       </c>
       <c r="B84" t="n">
-        <v>20141700122</v>
+        <v>20131700122</v>
       </c>
       <c r="C84" t="inlineStr">
         <is>
@@ -3240,7 +3241,7 @@
         <v>83</v>
       </c>
       <c r="B85" t="n">
-        <v>20030300123</v>
+        <v>20020300123</v>
       </c>
       <c r="C85" t="inlineStr">
         <is>
@@ -3265,7 +3266,7 @@
         <v>84</v>
       </c>
       <c r="B86" t="n">
-        <v>20122800124</v>
+        <v>20112800124</v>
       </c>
       <c r="C86" t="inlineStr">
         <is>
@@ -3290,7 +3291,7 @@
         <v>85</v>
       </c>
       <c r="B87" t="n">
-        <v>19991700125</v>
+        <v>19981700125</v>
       </c>
       <c r="C87" t="inlineStr">
         <is>
@@ -3315,7 +3316,7 @@
         <v>86</v>
       </c>
       <c r="B88" t="n">
-        <v>20160300126</v>
+        <v>20150300126</v>
       </c>
       <c r="C88" t="inlineStr">
         <is>
@@ -3340,7 +3341,7 @@
         <v>87</v>
       </c>
       <c r="B89" t="n">
-        <v>20201700127</v>
+        <v>20191700127</v>
       </c>
       <c r="C89" t="inlineStr">
         <is>
@@ -3365,7 +3366,7 @@
         <v>88</v>
       </c>
       <c r="B90" t="n">
-        <v>20110300128</v>
+        <v>20100300128</v>
       </c>
       <c r="C90" t="inlineStr">
         <is>
@@ -3390,7 +3391,7 @@
         <v>89</v>
       </c>
       <c r="B91" t="n">
-        <v>20132800129</v>
+        <v>20122800129</v>
       </c>
       <c r="C91" t="inlineStr">
         <is>
@@ -3415,7 +3416,7 @@
         <v>90</v>
       </c>
       <c r="B92" t="n">
-        <v>19950300130</v>
+        <v>19940300130</v>
       </c>
       <c r="C92" t="inlineStr">
         <is>
@@ -3440,7 +3441,7 @@
         <v>91</v>
       </c>
       <c r="B93" t="n">
-        <v>20140300131</v>
+        <v>20130300131</v>
       </c>
       <c r="C93" t="inlineStr">
         <is>
@@ -3465,7 +3466,7 @@
         <v>92</v>
       </c>
       <c r="B94" t="n">
-        <v>20000300132</v>
+        <v>19990300132</v>
       </c>
       <c r="C94" t="inlineStr">
         <is>
@@ -3490,7 +3491,7 @@
         <v>93</v>
       </c>
       <c r="B95" t="n">
-        <v>20170300133</v>
+        <v>20160300133</v>
       </c>
       <c r="C95" t="inlineStr">
         <is>
@@ -3515,7 +3516,7 @@
         <v>94</v>
       </c>
       <c r="B96" t="n">
-        <v>20130300134</v>
+        <v>20120300134</v>
       </c>
       <c r="C96" t="inlineStr">
         <is>
@@ -3540,7 +3541,7 @@
         <v>95</v>
       </c>
       <c r="B97" t="n">
-        <v>20011700135</v>
+        <v>20001700135</v>
       </c>
       <c r="C97" t="inlineStr">
         <is>
@@ -3565,7 +3566,7 @@
         <v>96</v>
       </c>
       <c r="B98" t="n">
-        <v>19960300136</v>
+        <v>19950300136</v>
       </c>
       <c r="C98" t="inlineStr">
         <is>
@@ -3590,7 +3591,7 @@
         <v>97</v>
       </c>
       <c r="B99" t="n">
-        <v>20130300137</v>
+        <v>20120300137</v>
       </c>
       <c r="C99" t="inlineStr">
         <is>
@@ -3615,7 +3616,7 @@
         <v>98</v>
       </c>
       <c r="B100" t="n">
-        <v>19950300138</v>
+        <v>19940300138</v>
       </c>
       <c r="C100" t="inlineStr">
         <is>
@@ -3640,7 +3641,7 @@
         <v>99</v>
       </c>
       <c r="B101" t="n">
-        <v>19842800139</v>
+        <v>19832800139</v>
       </c>
       <c r="C101" t="inlineStr">
         <is>
@@ -3665,7 +3666,7 @@
         <v>100</v>
       </c>
       <c r="B102" t="n">
-        <v>20182800140</v>
+        <v>20172800140</v>
       </c>
       <c r="C102" t="inlineStr">
         <is>
@@ -3690,7 +3691,7 @@
         <v>101</v>
       </c>
       <c r="B103" t="n">
-        <v>20031700141</v>
+        <v>20021700141</v>
       </c>
       <c r="C103" t="inlineStr">
         <is>
@@ -3715,7 +3716,7 @@
         <v>102</v>
       </c>
       <c r="B104" t="n">
-        <v>19981700142</v>
+        <v>19971700142</v>
       </c>
       <c r="C104" t="inlineStr">
         <is>
@@ -3740,7 +3741,7 @@
         <v>103</v>
       </c>
       <c r="B105" t="n">
-        <v>20090300143</v>
+        <v>20080300143</v>
       </c>
       <c r="C105" t="inlineStr">
         <is>
@@ -3765,7 +3766,7 @@
         <v>104</v>
       </c>
       <c r="B106" t="n">
-        <v>19921700144</v>
+        <v>19911700144</v>
       </c>
       <c r="C106" t="inlineStr">
         <is>
@@ -3790,7 +3791,7 @@
         <v>105</v>
       </c>
       <c r="B107" t="n">
-        <v>19922800146</v>
+        <v>19912800146</v>
       </c>
       <c r="C107" t="inlineStr">
         <is>
@@ -3815,7 +3816,7 @@
         <v>106</v>
       </c>
       <c r="B108" t="n">
-        <v>20162800147</v>
+        <v>20152800147</v>
       </c>
       <c r="C108" t="inlineStr">
         <is>
@@ -3840,7 +3841,7 @@
         <v>107</v>
       </c>
       <c r="B109" t="n">
-        <v>19872800148</v>
+        <v>19862800148</v>
       </c>
       <c r="C109" t="inlineStr">
         <is>
@@ -3865,7 +3866,7 @@
         <v>108</v>
       </c>
       <c r="B110" t="n">
-        <v>20061700149</v>
+        <v>20051700149</v>
       </c>
       <c r="C110" t="inlineStr">
         <is>
@@ -3890,7 +3891,7 @@
         <v>109</v>
       </c>
       <c r="B111" t="n">
-        <v>20061700150</v>
+        <v>20051700150</v>
       </c>
       <c r="C111" t="inlineStr">
         <is>
@@ -3915,7 +3916,7 @@
         <v>110</v>
       </c>
       <c r="B112" t="n">
-        <v>20021700151</v>
+        <v>20011700151</v>
       </c>
       <c r="C112" t="inlineStr">
         <is>
@@ -3940,7 +3941,7 @@
         <v>111</v>
       </c>
       <c r="B113" t="n">
-        <v>20121700152</v>
+        <v>20111700152</v>
       </c>
       <c r="C113" t="inlineStr">
         <is>
@@ -3965,7 +3966,7 @@
         <v>112</v>
       </c>
       <c r="B114" t="n">
-        <v>20010300153</v>
+        <v>20000300153</v>
       </c>
       <c r="C114" t="inlineStr">
         <is>
@@ -3990,7 +3991,7 @@
         <v>113</v>
       </c>
       <c r="B115" t="n">
-        <v>19990300154</v>
+        <v>19980300154</v>
       </c>
       <c r="C115" t="inlineStr">
         <is>
@@ -4015,7 +4016,7 @@
         <v>114</v>
       </c>
       <c r="B116" t="n">
-        <v>20072800155</v>
+        <v>20062800155</v>
       </c>
       <c r="C116" t="inlineStr">
         <is>
@@ -4040,7 +4041,7 @@
         <v>115</v>
       </c>
       <c r="B117" t="n">
-        <v>19982800156</v>
+        <v>19972800156</v>
       </c>
       <c r="C117" t="inlineStr">
         <is>
@@ -4065,7 +4066,7 @@
         <v>116</v>
       </c>
       <c r="B118" t="n">
-        <v>20172800157</v>
+        <v>20162800157</v>
       </c>
       <c r="C118" t="inlineStr">
         <is>
@@ -4090,7 +4091,7 @@
         <v>117</v>
       </c>
       <c r="B119" t="n">
-        <v>20201700158</v>
+        <v>20191700158</v>
       </c>
       <c r="C119" t="inlineStr">
         <is>
@@ -4115,7 +4116,7 @@
         <v>118</v>
       </c>
       <c r="B120" t="n">
-        <v>19970300159</v>
+        <v>19960300159</v>
       </c>
       <c r="C120" t="inlineStr">
         <is>
@@ -4140,7 +4141,7 @@
         <v>119</v>
       </c>
       <c r="B121" t="n">
-        <v>20001700160</v>
+        <v>19991700160</v>
       </c>
       <c r="C121" t="inlineStr">
         <is>
@@ -4165,7 +4166,7 @@
         <v>120</v>
       </c>
       <c r="B122" t="n">
-        <v>20020300161</v>
+        <v>20010300161</v>
       </c>
       <c r="C122" t="inlineStr">
         <is>
@@ -4190,7 +4191,7 @@
         <v>121</v>
       </c>
       <c r="B123" t="n">
-        <v>19892800162</v>
+        <v>19882800162</v>
       </c>
       <c r="C123" t="inlineStr">
         <is>
@@ -4215,7 +4216,7 @@
         <v>122</v>
       </c>
       <c r="B124" t="n">
-        <v>20101700165</v>
+        <v>20091700165</v>
       </c>
       <c r="C124" t="inlineStr">
         <is>
@@ -4240,7 +4241,7 @@
         <v>123</v>
       </c>
       <c r="B125" t="n">
-        <v>20133000166</v>
+        <v>20123000166</v>
       </c>
       <c r="C125" t="inlineStr">
         <is>
@@ -4265,7 +4266,7 @@
         <v>124</v>
       </c>
       <c r="B126" t="n">
-        <v>20173000167</v>
+        <v>20163000167</v>
       </c>
       <c r="C126" t="inlineStr">
         <is>
@@ -4290,7 +4291,7 @@
         <v>125</v>
       </c>
       <c r="B127" t="n">
-        <v>20201700168</v>
+        <v>20191700168</v>
       </c>
       <c r="C127" t="inlineStr">
         <is>
@@ -4315,7 +4316,7 @@
         <v>126</v>
       </c>
       <c r="B128" t="n">
-        <v>20043000170</v>
+        <v>20033000170</v>
       </c>
       <c r="C128" t="inlineStr">
         <is>
@@ -4340,7 +4341,7 @@
         <v>127</v>
       </c>
       <c r="B129" t="n">
-        <v>20153000171</v>
+        <v>20143000171</v>
       </c>
       <c r="C129" t="inlineStr">
         <is>
@@ -4365,7 +4366,7 @@
         <v>128</v>
       </c>
       <c r="B130" t="n">
-        <v>19852800172</v>
+        <v>19842800172</v>
       </c>
       <c r="C130" t="inlineStr">
         <is>
@@ -4390,7 +4391,7 @@
         <v>129</v>
       </c>
       <c r="B131" t="n">
-        <v>20110300173</v>
+        <v>20100300173</v>
       </c>
       <c r="C131" t="inlineStr">
         <is>
@@ -4415,7 +4416,7 @@
         <v>130</v>
       </c>
       <c r="B132" t="n">
-        <v>20173000174</v>
+        <v>20163000174</v>
       </c>
       <c r="C132" t="inlineStr">
         <is>
@@ -4440,7 +4441,7 @@
         <v>131</v>
       </c>
       <c r="B133" t="n">
-        <v>19923000175</v>
+        <v>19913000175</v>
       </c>
       <c r="C133" t="inlineStr">
         <is>
@@ -4465,7 +4466,7 @@
         <v>132</v>
       </c>
       <c r="B134" t="n">
-        <v>19951700176</v>
+        <v>19941700176</v>
       </c>
       <c r="C134" t="inlineStr">
         <is>
@@ -4490,7 +4491,7 @@
         <v>133</v>
       </c>
       <c r="B135" t="n">
-        <v>19831400177</v>
+        <v>19821400177</v>
       </c>
       <c r="C135" t="inlineStr">
         <is>
@@ -4515,7 +4516,7 @@
         <v>134</v>
       </c>
       <c r="B136" t="n">
-        <v>20053000178</v>
+        <v>20043000178</v>
       </c>
       <c r="C136" t="inlineStr">
         <is>
@@ -4540,7 +4541,7 @@
         <v>135</v>
       </c>
       <c r="B137" t="n">
-        <v>19872800180</v>
+        <v>19862800180</v>
       </c>
       <c r="C137" t="inlineStr">
         <is>
@@ -4565,7 +4566,7 @@
         <v>136</v>
       </c>
       <c r="B138" t="n">
-        <v>20142800181</v>
+        <v>20132800181</v>
       </c>
       <c r="C138" t="inlineStr">
         <is>
@@ -4590,7 +4591,7 @@
         <v>137</v>
       </c>
       <c r="B139" t="n">
-        <v>19882800182</v>
+        <v>19872800182</v>
       </c>
       <c r="C139" t="inlineStr">
         <is>
@@ -4615,7 +4616,7 @@
         <v>138</v>
       </c>
       <c r="B140" t="n">
-        <v>19822800183</v>
+        <v>19812800183</v>
       </c>
       <c r="C140" t="inlineStr">
         <is>
@@ -4640,7 +4641,7 @@
         <v>139</v>
       </c>
       <c r="B141" t="n">
-        <v>20181700184</v>
+        <v>20171700184</v>
       </c>
       <c r="C141" t="inlineStr">
         <is>
@@ -4665,7 +4666,7 @@
         <v>140</v>
       </c>
       <c r="B142" t="n">
-        <v>20152800185</v>
+        <v>20142800185</v>
       </c>
       <c r="C142" t="inlineStr">
         <is>
@@ -4690,7 +4691,7 @@
         <v>141</v>
       </c>
       <c r="B143" t="n">
-        <v>20132800186</v>
+        <v>20122800186</v>
       </c>
       <c r="C143" t="inlineStr">
         <is>
@@ -4715,7 +4716,7 @@
         <v>142</v>
       </c>
       <c r="B144" t="n">
-        <v>20082900187</v>
+        <v>20072900187</v>
       </c>
       <c r="C144" t="inlineStr">
         <is>
@@ -4740,7 +4741,7 @@
         <v>143</v>
       </c>
       <c r="B145" t="n">
-        <v>19942900188</v>
+        <v>19932900188</v>
       </c>
       <c r="C145" t="inlineStr">
         <is>
@@ -4765,7 +4766,7 @@
         <v>144</v>
       </c>
       <c r="B146" t="n">
-        <v>20052900189</v>
+        <v>20042900189</v>
       </c>
       <c r="C146" t="inlineStr">
         <is>
@@ -4790,7 +4791,7 @@
         <v>145</v>
       </c>
       <c r="B147" t="n">
-        <v>19862900190</v>
+        <v>19852900190</v>
       </c>
       <c r="C147" t="inlineStr">
         <is>
@@ -4815,7 +4816,7 @@
         <v>146</v>
       </c>
       <c r="B148" t="n">
-        <v>20102900191</v>
+        <v>20092900191</v>
       </c>
       <c r="C148" t="inlineStr">
         <is>
@@ -4840,7 +4841,7 @@
         <v>147</v>
       </c>
       <c r="B149" t="n">
-        <v>20122900192</v>
+        <v>20112900192</v>
       </c>
       <c r="C149" t="inlineStr">
         <is>
@@ -4865,7 +4866,7 @@
         <v>148</v>
       </c>
       <c r="B150" t="n">
-        <v>20010300193</v>
+        <v>20000300193</v>
       </c>
       <c r="C150" t="inlineStr">
         <is>
@@ -4890,7 +4891,7 @@
         <v>149</v>
       </c>
       <c r="B151" t="n">
-        <v>19952800194</v>
+        <v>19942800194</v>
       </c>
       <c r="C151" t="inlineStr">
         <is>
@@ -4915,7 +4916,7 @@
         <v>150</v>
       </c>
       <c r="B152" t="n">
-        <v>20062800195</v>
+        <v>20052800195</v>
       </c>
       <c r="C152" t="inlineStr">
         <is>
@@ -4940,7 +4941,7 @@
         <v>151</v>
       </c>
       <c r="B153" t="n">
-        <v>20123000196</v>
+        <v>20113000196</v>
       </c>
       <c r="C153" t="inlineStr">
         <is>
@@ -4965,7 +4966,7 @@
         <v>152</v>
       </c>
       <c r="B154" t="n">
-        <v>20083000197</v>
+        <v>20073000197</v>
       </c>
       <c r="C154" t="inlineStr">
         <is>
@@ -4990,7 +4991,7 @@
         <v>153</v>
       </c>
       <c r="B155" t="n">
-        <v>19912800198</v>
+        <v>19902800198</v>
       </c>
       <c r="C155" t="inlineStr">
         <is>
@@ -5015,7 +5016,7 @@
         <v>154</v>
       </c>
       <c r="B156" t="n">
-        <v>19992800199</v>
+        <v>19982800199</v>
       </c>
       <c r="C156" t="inlineStr">
         <is>
@@ -5040,7 +5041,7 @@
         <v>155</v>
       </c>
       <c r="B157" t="n">
-        <v>20172800200</v>
+        <v>20162800200</v>
       </c>
       <c r="C157" t="inlineStr">
         <is>
@@ -5065,7 +5066,7 @@
         <v>156</v>
       </c>
       <c r="B158" t="n">
-        <v>19942800201</v>
+        <v>19932800201</v>
       </c>
       <c r="C158" t="inlineStr">
         <is>
@@ -5090,7 +5091,7 @@
         <v>157</v>
       </c>
       <c r="B159" t="n">
-        <v>20102800202</v>
+        <v>20092800202</v>
       </c>
       <c r="C159" t="inlineStr">
         <is>
@@ -5115,7 +5116,7 @@
         <v>158</v>
       </c>
       <c r="B160" t="n">
-        <v>19962800203</v>
+        <v>19952800203</v>
       </c>
       <c r="C160" t="inlineStr">
         <is>
@@ -5140,7 +5141,7 @@
         <v>159</v>
       </c>
       <c r="B161" t="n">
-        <v>20011700204</v>
+        <v>20001700204</v>
       </c>
       <c r="C161" t="inlineStr">
         <is>
@@ -5165,7 +5166,7 @@
         <v>160</v>
       </c>
       <c r="B162" t="n">
-        <v>20152800205</v>
+        <v>20142800205</v>
       </c>
       <c r="C162" t="inlineStr">
         <is>
@@ -5190,7 +5191,7 @@
         <v>161</v>
       </c>
       <c r="B163" t="n">
-        <v>19861400207</v>
+        <v>19851400207</v>
       </c>
       <c r="C163" t="inlineStr">
         <is>
@@ -5215,7 +5216,7 @@
         <v>162</v>
       </c>
       <c r="B164" t="n">
-        <v>19851400208</v>
+        <v>19841400208</v>
       </c>
       <c r="C164" t="inlineStr">
         <is>
@@ -5240,7 +5241,7 @@
         <v>163</v>
       </c>
       <c r="B165" t="n">
-        <v>19881400209</v>
+        <v>19871400209</v>
       </c>
       <c r="C165" t="inlineStr">
         <is>
@@ -5265,7 +5266,7 @@
         <v>164</v>
       </c>
       <c r="B166" t="n">
-        <v>19901400210</v>
+        <v>19891400210</v>
       </c>
       <c r="C166" t="inlineStr">
         <is>
@@ -5290,7 +5291,7 @@
         <v>165</v>
       </c>
       <c r="B167" t="n">
-        <v>19970300211</v>
+        <v>19960300211</v>
       </c>
       <c r="C167" t="inlineStr">
         <is>
@@ -5315,7 +5316,7 @@
         <v>166</v>
       </c>
       <c r="B168" t="n">
-        <v>19992900212</v>
+        <v>19982900212</v>
       </c>
       <c r="C168" t="inlineStr">
         <is>
@@ -5340,7 +5341,7 @@
         <v>167</v>
       </c>
       <c r="B169" t="n">
-        <v>20010300213</v>
+        <v>20000300213</v>
       </c>
       <c r="C169" t="inlineStr">
         <is>
@@ -5365,7 +5366,7 @@
         <v>168</v>
       </c>
       <c r="B170" t="n">
-        <v>20030300214</v>
+        <v>20020300214</v>
       </c>
       <c r="C170" t="inlineStr">
         <is>
@@ -5390,7 +5391,7 @@
         <v>169</v>
       </c>
       <c r="B171" t="n">
-        <v>20132800216</v>
+        <v>20122800216</v>
       </c>
       <c r="C171" t="inlineStr">
         <is>
@@ -5415,7 +5416,7 @@
         <v>170</v>
       </c>
       <c r="B172" t="n">
-        <v>19982800217</v>
+        <v>19972800217</v>
       </c>
       <c r="C172" t="inlineStr">
         <is>
@@ -5440,7 +5441,7 @@
         <v>171</v>
       </c>
       <c r="B173" t="n">
-        <v>19822800218</v>
+        <v>19812800218</v>
       </c>
       <c r="C173" t="inlineStr">
         <is>
@@ -5465,7 +5466,7 @@
         <v>172</v>
       </c>
       <c r="B174" t="n">
-        <v>19862800219</v>
+        <v>19852800219</v>
       </c>
       <c r="C174" t="inlineStr">
         <is>
@@ -5490,7 +5491,7 @@
         <v>173</v>
       </c>
       <c r="B175" t="n">
-        <v>20150300220</v>
+        <v>20140300220</v>
       </c>
       <c r="C175" t="inlineStr">
         <is>
@@ -5515,7 +5516,7 @@
         <v>174</v>
       </c>
       <c r="B176" t="n">
-        <v>19950300221</v>
+        <v>19940300221</v>
       </c>
       <c r="C176" t="inlineStr">
         <is>
@@ -5540,7 +5541,7 @@
         <v>175</v>
       </c>
       <c r="B177" t="n">
-        <v>20201700222</v>
+        <v>20191700222</v>
       </c>
       <c r="C177" t="inlineStr">
         <is>
@@ -5565,7 +5566,7 @@
         <v>176</v>
       </c>
       <c r="B178" t="n">
-        <v>20070300223</v>
+        <v>20060300223</v>
       </c>
       <c r="C178" t="inlineStr">
         <is>
@@ -5590,7 +5591,7 @@
         <v>177</v>
       </c>
       <c r="B179" t="n">
-        <v>20051700224</v>
+        <v>20041700224</v>
       </c>
       <c r="C179" t="inlineStr">
         <is>
@@ -5615,7 +5616,7 @@
         <v>178</v>
       </c>
       <c r="B180" t="n">
-        <v>20120300225</v>
+        <v>20110300225</v>
       </c>
       <c r="C180" t="inlineStr">
         <is>
@@ -5640,7 +5641,7 @@
         <v>179</v>
       </c>
       <c r="B181" t="n">
-        <v>19912800226</v>
+        <v>19902800226</v>
       </c>
       <c r="C181" t="inlineStr">
         <is>
@@ -5665,7 +5666,7 @@
         <v>180</v>
       </c>
       <c r="B182" t="n">
-        <v>20050300227</v>
+        <v>20040300227</v>
       </c>
       <c r="C182" t="inlineStr">
         <is>
@@ -5690,7 +5691,7 @@
         <v>181</v>
       </c>
       <c r="B183" t="n">
-        <v>19963000228</v>
+        <v>19953000228</v>
       </c>
       <c r="C183" t="inlineStr">
         <is>
@@ -5715,7 +5716,7 @@
         <v>182</v>
       </c>
       <c r="B184" t="n">
-        <v>20073000229</v>
+        <v>20063000229</v>
       </c>
       <c r="C184" t="inlineStr">
         <is>
@@ -5740,7 +5741,7 @@
         <v>183</v>
       </c>
       <c r="B185" t="n">
-        <v>20140300230</v>
+        <v>20130300230</v>
       </c>
       <c r="C185" t="inlineStr">
         <is>
@@ -5765,7 +5766,7 @@
         <v>184</v>
       </c>
       <c r="B186" t="n">
-        <v>20183000232</v>
+        <v>20173000232</v>
       </c>
       <c r="C186" t="inlineStr">
         <is>
@@ -5790,7 +5791,7 @@
         <v>185</v>
       </c>
       <c r="B187" t="n">
-        <v>19912800233</v>
+        <v>19902800233</v>
       </c>
       <c r="C187" t="inlineStr">
         <is>
@@ -5815,7 +5816,7 @@
         <v>186</v>
       </c>
       <c r="B188" t="n">
-        <v>19962800234</v>
+        <v>19952800234</v>
       </c>
       <c r="C188" t="inlineStr">
         <is>
@@ -5840,7 +5841,7 @@
         <v>187</v>
       </c>
       <c r="B189" t="n">
-        <v>20073000235</v>
+        <v>20063000235</v>
       </c>
       <c r="C189" t="inlineStr">
         <is>
@@ -5865,7 +5866,7 @@
         <v>188</v>
       </c>
       <c r="B190" t="n">
-        <v>20172800236</v>
+        <v>20162800236</v>
       </c>
       <c r="C190" t="inlineStr">
         <is>
@@ -5890,7 +5891,7 @@
         <v>189</v>
       </c>
       <c r="B191" t="n">
-        <v>19992800237</v>
+        <v>19982800237</v>
       </c>
       <c r="C191" t="inlineStr">
         <is>
@@ -5915,7 +5916,7 @@
         <v>190</v>
       </c>
       <c r="B192" t="n">
-        <v>19941700239</v>
+        <v>19931700239</v>
       </c>
       <c r="C192" t="inlineStr">
         <is>
@@ -5940,7 +5941,7 @@
         <v>191</v>
       </c>
       <c r="B193" t="n">
-        <v>20101700240</v>
+        <v>20091700240</v>
       </c>
       <c r="C193" t="inlineStr">
         <is>
@@ -5965,7 +5966,7 @@
         <v>192</v>
       </c>
       <c r="B194" t="n">
-        <v>20201700241</v>
+        <v>20191700241</v>
       </c>
       <c r="C194" t="inlineStr">
         <is>
@@ -5990,7 +5991,7 @@
         <v>193</v>
       </c>
       <c r="B195" t="n">
-        <v>20121700242</v>
+        <v>20111700242</v>
       </c>
       <c r="C195" t="inlineStr">
         <is>
@@ -6015,7 +6016,7 @@
         <v>194</v>
       </c>
       <c r="B196" t="n">
-        <v>19842900243</v>
+        <v>19832900243</v>
       </c>
       <c r="C196" t="inlineStr">
         <is>
@@ -6040,7 +6041,7 @@
         <v>195</v>
       </c>
       <c r="B197" t="n">
-        <v>20100300245</v>
+        <v>20090300245</v>
       </c>
       <c r="C197" t="inlineStr">
         <is>
@@ -6065,7 +6066,7 @@
         <v>196</v>
       </c>
       <c r="B198" t="n">
-        <v>19832800246</v>
+        <v>19822800246</v>
       </c>
       <c r="C198" t="inlineStr">
         <is>
@@ -6090,7 +6091,7 @@
         <v>197</v>
       </c>
       <c r="B199" t="n">
-        <v>19992800247</v>
+        <v>19982800247</v>
       </c>
       <c r="C199" t="inlineStr">
         <is>
@@ -6115,7 +6116,7 @@
         <v>198</v>
       </c>
       <c r="B200" t="n">
-        <v>20172800248</v>
+        <v>20162800248</v>
       </c>
       <c r="C200" t="inlineStr">
         <is>
@@ -6140,7 +6141,7 @@
         <v>199</v>
       </c>
       <c r="B201" t="n">
-        <v>19992800249</v>
+        <v>19982800249</v>
       </c>
       <c r="C201" t="inlineStr">
         <is>
@@ -6165,7 +6166,7 @@
         <v>200</v>
       </c>
       <c r="B202" t="n">
-        <v>20022900251</v>
+        <v>20012900251</v>
       </c>
       <c r="C202" t="inlineStr">
         <is>
@@ -6190,7 +6191,7 @@
         <v>201</v>
       </c>
       <c r="B203" t="n">
-        <v>19862900252</v>
+        <v>19852900252</v>
       </c>
       <c r="C203" t="inlineStr">
         <is>
@@ -6215,7 +6216,7 @@
         <v>202</v>
       </c>
       <c r="B204" t="n">
-        <v>20082900253</v>
+        <v>20072900253</v>
       </c>
       <c r="C204" t="inlineStr">
         <is>
@@ -6240,7 +6241,7 @@
         <v>203</v>
       </c>
       <c r="B205" t="n">
-        <v>19952900254</v>
+        <v>19942900254</v>
       </c>
       <c r="C205" t="inlineStr">
         <is>
@@ -6265,7 +6266,7 @@
         <v>204</v>
       </c>
       <c r="B206" t="n">
-        <v>19842900255</v>
+        <v>19832900255</v>
       </c>
       <c r="C206" t="inlineStr">
         <is>
@@ -6290,7 +6291,7 @@
         <v>205</v>
       </c>
       <c r="B207" t="n">
-        <v>20182900256</v>
+        <v>20172900256</v>
       </c>
       <c r="C207" t="inlineStr">
         <is>
@@ -6315,7 +6316,7 @@
         <v>206</v>
       </c>
       <c r="B208" t="n">
-        <v>19832900257</v>
+        <v>19822900257</v>
       </c>
       <c r="C208" t="inlineStr">
         <is>
@@ -6340,7 +6341,7 @@
         <v>207</v>
       </c>
       <c r="B209" t="n">
-        <v>20092900258</v>
+        <v>20082900258</v>
       </c>
       <c r="C209" t="inlineStr">
         <is>
@@ -6365,7 +6366,7 @@
         <v>208</v>
       </c>
       <c r="B210" t="n">
-        <v>19822900259</v>
+        <v>19812900259</v>
       </c>
       <c r="C210" t="inlineStr">
         <is>
@@ -6390,7 +6391,7 @@
         <v>209</v>
       </c>
       <c r="B211" t="n">
-        <v>20022900260</v>
+        <v>20012900260</v>
       </c>
       <c r="C211" t="inlineStr">
         <is>
@@ -6415,7 +6416,7 @@
         <v>210</v>
       </c>
       <c r="B212" t="n">
-        <v>20162900261</v>
+        <v>20152900261</v>
       </c>
       <c r="C212" t="inlineStr">
         <is>
@@ -6440,7 +6441,7 @@
         <v>211</v>
       </c>
       <c r="B213" t="n">
-        <v>20172900262</v>
+        <v>20162900262</v>
       </c>
       <c r="C213" t="inlineStr">
         <is>
@@ -6465,7 +6466,7 @@
         <v>212</v>
       </c>
       <c r="B214" t="n">
-        <v>19902900263</v>
+        <v>19892900263</v>
       </c>
       <c r="C214" t="inlineStr">
         <is>
@@ -6490,7 +6491,7 @@
         <v>213</v>
       </c>
       <c r="B215" t="n">
-        <v>19992900264</v>
+        <v>19982900264</v>
       </c>
       <c r="C215" t="inlineStr">
         <is>
@@ -6515,7 +6516,7 @@
         <v>214</v>
       </c>
       <c r="B216" t="n">
-        <v>19912800265</v>
+        <v>19902800265</v>
       </c>
       <c r="C216" t="inlineStr">
         <is>
@@ -6540,7 +6541,7 @@
         <v>215</v>
       </c>
       <c r="B217" t="n">
-        <v>20170300266</v>
+        <v>20160300266</v>
       </c>
       <c r="C217" t="inlineStr">
         <is>
@@ -6565,7 +6566,7 @@
         <v>216</v>
       </c>
       <c r="B218" t="n">
-        <v>19941700298</v>
+        <v>19931700298</v>
       </c>
       <c r="C218" t="inlineStr">
         <is>
@@ -6590,7 +6591,7 @@
         <v>217</v>
       </c>
       <c r="B219" t="n">
-        <v>19993000314</v>
+        <v>19983000314</v>
       </c>
       <c r="C219" t="inlineStr">
         <is>
@@ -6615,7 +6616,7 @@
         <v>218</v>
       </c>
       <c r="B220" t="n">
-        <v>19923000315</v>
+        <v>19913000315</v>
       </c>
       <c r="C220" t="inlineStr">
         <is>
@@ -6640,7 +6641,7 @@
         <v>219</v>
       </c>
       <c r="B221" t="n">
-        <v>20132800316</v>
+        <v>20122800316</v>
       </c>
       <c r="C221" t="inlineStr">
         <is>
@@ -6665,7 +6666,7 @@
         <v>220</v>
       </c>
       <c r="B222" t="n">
-        <v>20052800317</v>
+        <v>20042800317</v>
       </c>
       <c r="C222" t="inlineStr">
         <is>
@@ -6690,7 +6691,7 @@
         <v>221</v>
       </c>
       <c r="B223" t="n">
-        <v>20162800318</v>
+        <v>20152800318</v>
       </c>
       <c r="C223" t="inlineStr">
         <is>
@@ -6715,7 +6716,7 @@
         <v>222</v>
       </c>
       <c r="B224" t="n">
-        <v>19892800319</v>
+        <v>19882800319</v>
       </c>
       <c r="C224" t="inlineStr">
         <is>
@@ -6740,7 +6741,7 @@
         <v>223</v>
       </c>
       <c r="B225" t="n">
-        <v>19892800320</v>
+        <v>19882800320</v>
       </c>
       <c r="C225" t="inlineStr">
         <is>
@@ -6765,7 +6766,7 @@
         <v>224</v>
       </c>
       <c r="B226" t="n">
-        <v>20040300321</v>
+        <v>20030300321</v>
       </c>
       <c r="C226" t="inlineStr">
         <is>
@@ -6790,7 +6791,7 @@
         <v>225</v>
       </c>
       <c r="B227" t="n">
-        <v>20092900323</v>
+        <v>20082900323</v>
       </c>
       <c r="C227" t="inlineStr">
         <is>
@@ -6815,7 +6816,7 @@
         <v>226</v>
       </c>
       <c r="B228" t="n">
-        <v>20032900324</v>
+        <v>20022900324</v>
       </c>
       <c r="C228" t="inlineStr">
         <is>
@@ -6840,7 +6841,7 @@
         <v>227</v>
       </c>
       <c r="B229" t="n">
-        <v>20132800325</v>
+        <v>20122800325</v>
       </c>
       <c r="C229" t="inlineStr">
         <is>
@@ -6865,7 +6866,7 @@
         <v>228</v>
       </c>
       <c r="B230" t="n">
-        <v>19922800326</v>
+        <v>19912800326</v>
       </c>
       <c r="C230" t="inlineStr">
         <is>
@@ -6890,7 +6891,7 @@
         <v>229</v>
       </c>
       <c r="B231" t="n">
-        <v>19842900327</v>
+        <v>19832900327</v>
       </c>
       <c r="C231" t="inlineStr">
         <is>
@@ -6915,7 +6916,7 @@
         <v>230</v>
       </c>
       <c r="B232" t="n">
-        <v>19822900328</v>
+        <v>19812900328</v>
       </c>
       <c r="C232" t="inlineStr">
         <is>
@@ -6940,7 +6941,7 @@
         <v>231</v>
       </c>
       <c r="B233" t="n">
-        <v>20042800331</v>
+        <v>20032800331</v>
       </c>
       <c r="C233" t="inlineStr">
         <is>
@@ -6965,7 +6966,7 @@
         <v>232</v>
       </c>
       <c r="B234" t="n">
-        <v>20063000332</v>
+        <v>20053000332</v>
       </c>
       <c r="C234" t="inlineStr">
         <is>
@@ -6990,7 +6991,7 @@
         <v>233</v>
       </c>
       <c r="B235" t="n">
-        <v>20173000333</v>
+        <v>20163000333</v>
       </c>
       <c r="C235" t="inlineStr">
         <is>
@@ -7015,7 +7016,7 @@
         <v>234</v>
       </c>
       <c r="B236" t="n">
-        <v>19973000334</v>
+        <v>19963000334</v>
       </c>
       <c r="C236" t="inlineStr">
         <is>
@@ -7040,7 +7041,7 @@
         <v>235</v>
       </c>
       <c r="B237" t="n">
-        <v>20071700336</v>
+        <v>20061700336</v>
       </c>
       <c r="C237" t="inlineStr">
         <is>
@@ -7065,7 +7066,7 @@
         <v>236</v>
       </c>
       <c r="B238" t="n">
-        <v>20071700337</v>
+        <v>20061700337</v>
       </c>
       <c r="C238" t="inlineStr">
         <is>
@@ -7090,7 +7091,7 @@
         <v>237</v>
       </c>
       <c r="B239" t="n">
-        <v>20111700338</v>
+        <v>20101700338</v>
       </c>
       <c r="C239" t="inlineStr">
         <is>
@@ -7115,7 +7116,7 @@
         <v>238</v>
       </c>
       <c r="B240" t="n">
-        <v>20091700339</v>
+        <v>20081700339</v>
       </c>
       <c r="C240" t="inlineStr">
         <is>
@@ -7140,7 +7141,7 @@
         <v>239</v>
       </c>
       <c r="B241" t="n">
-        <v>20071700340</v>
+        <v>20061700340</v>
       </c>
       <c r="C241" t="inlineStr">
         <is>
@@ -7165,7 +7166,7 @@
         <v>240</v>
       </c>
       <c r="B242" t="n">
-        <v>20051700341</v>
+        <v>20041700341</v>
       </c>
       <c r="C242" t="inlineStr">
         <is>
@@ -7190,7 +7191,7 @@
         <v>241</v>
       </c>
       <c r="B243" t="n">
-        <v>20031700342</v>
+        <v>20021700342</v>
       </c>
       <c r="C243" t="inlineStr">
         <is>
@@ -7215,7 +7216,7 @@
         <v>242</v>
       </c>
       <c r="B244" t="n">
-        <v>20043000363</v>
+        <v>20033000363</v>
       </c>
       <c r="C244" t="inlineStr">
         <is>
@@ -7240,7 +7241,7 @@
         <v>243</v>
       </c>
       <c r="B245" t="n">
-        <v>20092800364</v>
+        <v>20082800364</v>
       </c>
       <c r="C245" t="inlineStr">
         <is>
@@ -7265,7 +7266,7 @@
         <v>244</v>
       </c>
       <c r="B246" t="n">
-        <v>19941700365</v>
+        <v>19931700365</v>
       </c>
       <c r="C246" t="inlineStr">
         <is>
@@ -7290,7 +7291,7 @@
         <v>245</v>
       </c>
       <c r="B247" t="n">
-        <v>20080300367</v>
+        <v>20070300367</v>
       </c>
       <c r="C247" t="inlineStr">
         <is>
@@ -7315,7 +7316,7 @@
         <v>246</v>
       </c>
       <c r="B248" t="n">
-        <v>20010300368</v>
+        <v>20000300368</v>
       </c>
       <c r="C248" t="inlineStr">
         <is>
@@ -7340,7 +7341,7 @@
         <v>247</v>
       </c>
       <c r="B249" t="n">
-        <v>20060300369</v>
+        <v>20050300369</v>
       </c>
       <c r="C249" t="inlineStr">
         <is>
@@ -7365,7 +7366,7 @@
         <v>248</v>
       </c>
       <c r="B250" t="n">
-        <v>20160300370</v>
+        <v>20150300370</v>
       </c>
       <c r="C250" t="inlineStr">
         <is>
@@ -7390,7 +7391,7 @@
         <v>249</v>
       </c>
       <c r="B251" t="n">
-        <v>19980300371</v>
+        <v>19970300371</v>
       </c>
       <c r="C251" t="inlineStr">
         <is>
@@ -7415,7 +7416,7 @@
         <v>250</v>
       </c>
       <c r="B252" t="n">
-        <v>20070300372</v>
+        <v>20060300372</v>
       </c>
       <c r="C252" t="inlineStr">
         <is>
@@ -7440,7 +7441,7 @@
         <v>251</v>
       </c>
       <c r="B253" t="n">
-        <v>20132800373</v>
+        <v>20122800373</v>
       </c>
       <c r="C253" t="inlineStr">
         <is>
@@ -7465,7 +7466,7 @@
         <v>252</v>
       </c>
       <c r="B254" t="n">
-        <v>20020300374</v>
+        <v>20010300374</v>
       </c>
       <c r="C254" t="inlineStr">
         <is>
@@ -7490,7 +7491,7 @@
         <v>253</v>
       </c>
       <c r="B255" t="n">
-        <v>19920300375</v>
+        <v>19910300375</v>
       </c>
       <c r="C255" t="inlineStr">
         <is>
@@ -7515,7 +7516,7 @@
         <v>254</v>
       </c>
       <c r="B256" t="n">
-        <v>19912800376</v>
+        <v>19902800376</v>
       </c>
       <c r="C256" t="inlineStr">
         <is>
@@ -7540,7 +7541,7 @@
         <v>255</v>
       </c>
       <c r="B257" t="n">
-        <v>20011700378</v>
+        <v>20001700378</v>
       </c>
       <c r="C257" t="inlineStr">
         <is>
@@ -7565,7 +7566,7 @@
         <v>256</v>
       </c>
       <c r="B258" t="n">
-        <v>19940300379</v>
+        <v>19930300379</v>
       </c>
       <c r="C258" t="inlineStr">
         <is>
@@ -7590,7 +7591,7 @@
         <v>257</v>
       </c>
       <c r="B259" t="n">
-        <v>20002800383</v>
+        <v>19992800383</v>
       </c>
       <c r="C259" t="inlineStr">
         <is>
@@ -7615,7 +7616,7 @@
         <v>258</v>
       </c>
       <c r="B260" t="n">
-        <v>19872800384</v>
+        <v>19862800384</v>
       </c>
       <c r="C260" t="inlineStr">
         <is>
@@ -7640,7 +7641,7 @@
         <v>259</v>
       </c>
       <c r="B261" t="n">
-        <v>20182800386</v>
+        <v>20172800386</v>
       </c>
       <c r="C261" t="inlineStr">
         <is>
@@ -7665,7 +7666,7 @@
         <v>260</v>
       </c>
       <c r="B262" t="n">
-        <v>20022900387</v>
+        <v>20012900387</v>
       </c>
       <c r="C262" t="inlineStr">
         <is>
@@ -7690,7 +7691,7 @@
         <v>261</v>
       </c>
       <c r="B263" t="n">
-        <v>20102900388</v>
+        <v>20092900388</v>
       </c>
       <c r="C263" t="inlineStr">
         <is>
@@ -7715,7 +7716,7 @@
         <v>262</v>
       </c>
       <c r="B264" t="n">
-        <v>19852900389</v>
+        <v>19842900389</v>
       </c>
       <c r="C264" t="inlineStr">
         <is>
@@ -7740,7 +7741,7 @@
         <v>263</v>
       </c>
       <c r="B265" t="n">
-        <v>20022900390</v>
+        <v>20012900390</v>
       </c>
       <c r="C265" t="inlineStr">
         <is>
@@ -7765,7 +7766,7 @@
         <v>264</v>
       </c>
       <c r="B266" t="n">
-        <v>19961700391</v>
+        <v>19951700391</v>
       </c>
       <c r="C266" t="inlineStr">
         <is>
@@ -7790,7 +7791,7 @@
         <v>265</v>
       </c>
       <c r="B267" t="n">
-        <v>20191700392</v>
+        <v>20181700392</v>
       </c>
       <c r="C267" t="inlineStr">
         <is>
@@ -7815,7 +7816,7 @@
         <v>266</v>
       </c>
       <c r="B268" t="n">
-        <v>20172800394</v>
+        <v>20162800394</v>
       </c>
       <c r="C268" t="inlineStr">
         <is>
@@ -7840,7 +7841,7 @@
         <v>267</v>
       </c>
       <c r="B269" t="n">
-        <v>20042800395</v>
+        <v>20032800395</v>
       </c>
       <c r="C269" t="inlineStr">
         <is>
@@ -7865,7 +7866,7 @@
         <v>268</v>
       </c>
       <c r="B270" t="n">
-        <v>20032800396</v>
+        <v>20022800396</v>
       </c>
       <c r="C270" t="inlineStr">
         <is>
@@ -7890,7 +7891,7 @@
         <v>269</v>
       </c>
       <c r="B271" t="n">
-        <v>20033000397</v>
+        <v>20023000397</v>
       </c>
       <c r="C271" t="inlineStr">
         <is>
@@ -7915,7 +7916,7 @@
         <v>270</v>
       </c>
       <c r="B272" t="n">
-        <v>19941700398</v>
+        <v>19931700398</v>
       </c>
       <c r="C272" t="inlineStr">
         <is>
@@ -7940,7 +7941,7 @@
         <v>271</v>
       </c>
       <c r="B273" t="n">
-        <v>20052800400</v>
+        <v>20042800400</v>
       </c>
       <c r="C273" t="inlineStr">
         <is>
@@ -8026,7 +8027,7 @@
         <v>0</v>
       </c>
       <c r="B2" t="n">
-        <v>19721200050</v>
+        <v>19711200050</v>
       </c>
       <c r="C2" t="n">
         <v>79.8</v>
@@ -8065,7 +8066,7 @@
         <v>1</v>
       </c>
       <c r="B3" t="n">
-        <v>19981200057</v>
+        <v>19971200057</v>
       </c>
       <c r="C3" t="n">
         <v>50</v>
@@ -8104,7 +8105,7 @@
         <v>2</v>
       </c>
       <c r="B4" t="n">
-        <v>19881200080</v>
+        <v>19871200080</v>
       </c>
       <c r="C4" t="n">
         <v>220</v>
@@ -8143,7 +8144,7 @@
         <v>3</v>
       </c>
       <c r="B5" t="n">
-        <v>20041200100</v>
+        <v>20031200100</v>
       </c>
       <c r="C5" t="n">
         <v>119.1</v>
@@ -8182,7 +8183,7 @@
         <v>4</v>
       </c>
       <c r="B6" t="n">
-        <v>20081200110</v>
+        <v>20071200110</v>
       </c>
       <c r="C6" t="n">
         <v>1052</v>
@@ -8221,7 +8222,7 @@
         <v>5</v>
       </c>
       <c r="B7" t="n">
-        <v>19971200145</v>
+        <v>19961200145</v>
       </c>
       <c r="C7" t="n">
         <v>160</v>
@@ -8260,7 +8261,7 @@
         <v>6</v>
       </c>
       <c r="B8" t="n">
-        <v>19991200163</v>
+        <v>19981200163</v>
       </c>
       <c r="C8" t="n">
         <v>59.8</v>
@@ -8299,7 +8300,7 @@
         <v>7</v>
       </c>
       <c r="B9" t="n">
-        <v>19741200164</v>
+        <v>19731200164</v>
       </c>
       <c r="C9" t="n">
         <v>317.8</v>
@@ -8338,7 +8339,7 @@
         <v>8</v>
       </c>
       <c r="B10" t="n">
-        <v>19781200169</v>
+        <v>19771200169</v>
       </c>
       <c r="C10" t="n">
         <v>100</v>
@@ -8377,7 +8378,7 @@
         <v>9</v>
       </c>
       <c r="B11" t="n">
-        <v>19881200179</v>
+        <v>19871200179</v>
       </c>
       <c r="C11" t="n">
         <v>66</v>
@@ -8416,7 +8417,7 @@
         <v>10</v>
       </c>
       <c r="B12" t="n">
-        <v>19761200206</v>
+        <v>19751200206</v>
       </c>
       <c r="C12" t="n">
         <v>53.7</v>
@@ -8455,7 +8456,7 @@
         <v>11</v>
       </c>
       <c r="B13" t="n">
-        <v>19811200215</v>
+        <v>19801200215</v>
       </c>
       <c r="C13" t="n">
         <v>153</v>
@@ -8494,7 +8495,7 @@
         <v>12</v>
       </c>
       <c r="B14" t="n">
-        <v>19871200231</v>
+        <v>19861200231</v>
       </c>
       <c r="C14" t="n">
         <v>150</v>
@@ -8533,7 +8534,7 @@
         <v>13</v>
       </c>
       <c r="B15" t="n">
-        <v>20041200238</v>
+        <v>20031200238</v>
       </c>
       <c r="C15" t="n">
         <v>99</v>
@@ -8572,7 +8573,7 @@
         <v>14</v>
       </c>
       <c r="B16" t="n">
-        <v>20031200244</v>
+        <v>20021200244</v>
       </c>
       <c r="C16" t="n">
         <v>1045.2</v>
@@ -8611,7 +8612,7 @@
         <v>15</v>
       </c>
       <c r="B17" t="n">
-        <v>20172300267</v>
+        <v>20162300267</v>
       </c>
       <c r="C17" t="n">
         <v>500</v>
@@ -8650,7 +8651,7 @@
         <v>16</v>
       </c>
       <c r="B18" t="n">
-        <v>20172300268</v>
+        <v>20162300268</v>
       </c>
       <c r="C18" t="n">
         <v>500</v>
@@ -8689,7 +8690,7 @@
         <v>17</v>
       </c>
       <c r="B19" t="n">
-        <v>20192300269</v>
+        <v>20182300269</v>
       </c>
       <c r="C19" t="n">
         <v>500</v>
@@ -8728,7 +8729,7 @@
         <v>18</v>
       </c>
       <c r="B20" t="n">
-        <v>20152300270</v>
+        <v>20142300270</v>
       </c>
       <c r="C20" t="n">
         <v>500</v>
@@ -8767,7 +8768,7 @@
         <v>19</v>
       </c>
       <c r="B21" t="n">
-        <v>20172300271</v>
+        <v>20162300271</v>
       </c>
       <c r="C21" t="n">
         <v>500</v>
@@ -8806,7 +8807,7 @@
         <v>20</v>
       </c>
       <c r="B22" t="n">
-        <v>20152300272</v>
+        <v>20142300272</v>
       </c>
       <c r="C22" t="n">
         <v>500</v>
@@ -8845,7 +8846,7 @@
         <v>21</v>
       </c>
       <c r="B23" t="n">
-        <v>20092400273</v>
+        <v>20082400273</v>
       </c>
       <c r="C23" t="n">
         <v>1815</v>
@@ -8884,7 +8885,7 @@
         <v>22</v>
       </c>
       <c r="B24" t="n">
-        <v>20152400274</v>
+        <v>20142400274</v>
       </c>
       <c r="C24" t="n">
         <v>1815</v>
@@ -8923,7 +8924,7 @@
         <v>23</v>
       </c>
       <c r="B25" t="n">
-        <v>20122400275</v>
+        <v>20112400275</v>
       </c>
       <c r="C25" t="n">
         <v>1815</v>
@@ -8962,7 +8963,7 @@
         <v>24</v>
       </c>
       <c r="B26" t="n">
-        <v>20122400276</v>
+        <v>20112400276</v>
       </c>
       <c r="C26" t="n">
         <v>1815</v>
@@ -9001,7 +9002,7 @@
         <v>25</v>
       </c>
       <c r="B27" t="n">
-        <v>20202400277</v>
+        <v>20192400277</v>
       </c>
       <c r="C27" t="n">
         <v>1815</v>
@@ -9040,7 +9041,7 @@
         <v>26</v>
       </c>
       <c r="B28" t="n">
-        <v>20142400278</v>
+        <v>20132400278</v>
       </c>
       <c r="C28" t="n">
         <v>1815</v>
@@ -9079,7 +9080,7 @@
         <v>27</v>
       </c>
       <c r="B29" t="n">
-        <v>20182400279</v>
+        <v>20172400279</v>
       </c>
       <c r="C29" t="n">
         <v>1815</v>
@@ -9118,7 +9119,7 @@
         <v>28</v>
       </c>
       <c r="B30" t="n">
-        <v>20182400280</v>
+        <v>20172400280</v>
       </c>
       <c r="C30" t="n">
         <v>1815</v>
@@ -9157,7 +9158,7 @@
         <v>29</v>
       </c>
       <c r="B31" t="n">
-        <v>20092400281</v>
+        <v>20082400281</v>
       </c>
       <c r="C31" t="n">
         <v>1815</v>
@@ -9196,7 +9197,7 @@
         <v>30</v>
       </c>
       <c r="B32" t="n">
-        <v>20112400282</v>
+        <v>20102400282</v>
       </c>
       <c r="C32" t="n">
         <v>1815</v>
@@ -9235,7 +9236,7 @@
         <v>31</v>
       </c>
       <c r="B33" t="n">
-        <v>20102400283</v>
+        <v>20092400283</v>
       </c>
       <c r="C33" t="n">
         <v>1815</v>
@@ -9274,7 +9275,7 @@
         <v>32</v>
       </c>
       <c r="B34" t="n">
-        <v>20192400284</v>
+        <v>20182400284</v>
       </c>
       <c r="C34" t="n">
         <v>1815</v>
@@ -9313,7 +9314,7 @@
         <v>33</v>
       </c>
       <c r="B35" t="n">
-        <v>20132400285</v>
+        <v>20122400285</v>
       </c>
       <c r="C35" t="n">
         <v>1815</v>
@@ -9352,7 +9353,7 @@
         <v>34</v>
       </c>
       <c r="B36" t="n">
-        <v>20102400286</v>
+        <v>20092400286</v>
       </c>
       <c r="C36" t="n">
         <v>1000</v>
@@ -9391,7 +9392,7 @@
         <v>35</v>
       </c>
       <c r="B37" t="n">
-        <v>20082400287</v>
+        <v>20072400287</v>
       </c>
       <c r="C37" t="n">
         <v>1000</v>
@@ -9430,7 +9431,7 @@
         <v>36</v>
       </c>
       <c r="B38" t="n">
-        <v>20062400288</v>
+        <v>20052400288</v>
       </c>
       <c r="C38" t="n">
         <v>1000</v>
@@ -9469,7 +9470,7 @@
         <v>37</v>
       </c>
       <c r="B39" t="n">
-        <v>20122400289</v>
+        <v>20112400289</v>
       </c>
       <c r="C39" t="n">
         <v>1000</v>
@@ -9508,7 +9509,7 @@
         <v>38</v>
       </c>
       <c r="B40" t="n">
-        <v>20142400290</v>
+        <v>20132400290</v>
       </c>
       <c r="C40" t="n">
         <v>1000</v>
@@ -9547,7 +9548,7 @@
         <v>39</v>
       </c>
       <c r="B41" t="n">
-        <v>20182400291</v>
+        <v>20172400291</v>
       </c>
       <c r="C41" t="n">
         <v>1815</v>
@@ -9586,7 +9587,7 @@
         <v>40</v>
       </c>
       <c r="B42" t="n">
-        <v>20192400292</v>
+        <v>20182400292</v>
       </c>
       <c r="C42" t="n">
         <v>1815</v>
@@ -9625,7 +9626,7 @@
         <v>41</v>
       </c>
       <c r="B43" t="n">
-        <v>20152400293</v>
+        <v>20142400293</v>
       </c>
       <c r="C43" t="n">
         <v>1815</v>
@@ -9664,7 +9665,7 @@
         <v>42</v>
       </c>
       <c r="B44" t="n">
-        <v>20092400294</v>
+        <v>20082400294</v>
       </c>
       <c r="C44" t="n">
         <v>1815</v>
@@ -9703,7 +9704,7 @@
         <v>43</v>
       </c>
       <c r="B45" t="n">
-        <v>20162400295</v>
+        <v>20152400295</v>
       </c>
       <c r="C45" t="n">
         <v>1815</v>
@@ -9742,7 +9743,7 @@
         <v>44</v>
       </c>
       <c r="B46" t="n">
-        <v>20122400296</v>
+        <v>20112400296</v>
       </c>
       <c r="C46" t="n">
         <v>1815</v>
@@ -9781,7 +9782,7 @@
         <v>45</v>
       </c>
       <c r="B47" t="n">
-        <v>20132400297</v>
+        <v>20122400297</v>
       </c>
       <c r="C47" t="n">
         <v>1815</v>
@@ -9820,7 +9821,7 @@
         <v>46</v>
       </c>
       <c r="B48" t="n">
-        <v>19951200299</v>
+        <v>19941200299</v>
       </c>
       <c r="C48" t="n">
         <v>164</v>
@@ -9859,7 +9860,7 @@
         <v>47</v>
       </c>
       <c r="B49" t="n">
-        <v>19771200300</v>
+        <v>19761200300</v>
       </c>
       <c r="C49" t="n">
         <v>196</v>
@@ -9898,7 +9899,7 @@
         <v>48</v>
       </c>
       <c r="B50" t="n">
-        <v>20091200301</v>
+        <v>20081200301</v>
       </c>
       <c r="C50" t="n">
         <v>100</v>
@@ -9937,7 +9938,7 @@
         <v>49</v>
       </c>
       <c r="B51" t="n">
-        <v>19851200302</v>
+        <v>19841200302</v>
       </c>
       <c r="C51" t="n">
         <v>100</v>
@@ -9976,7 +9977,7 @@
         <v>50</v>
       </c>
       <c r="B52" t="n">
-        <v>19861200303</v>
+        <v>19851200303</v>
       </c>
       <c r="C52" t="n">
         <v>195</v>
@@ -10015,7 +10016,7 @@
         <v>51</v>
       </c>
       <c r="B53" t="n">
-        <v>20081200304</v>
+        <v>20071200304</v>
       </c>
       <c r="C53" t="n">
         <v>100</v>
@@ -10054,7 +10055,7 @@
         <v>52</v>
       </c>
       <c r="B54" t="n">
-        <v>19931200305</v>
+        <v>19921200305</v>
       </c>
       <c r="C54" t="n">
         <v>100</v>
@@ -10093,7 +10094,7 @@
         <v>53</v>
       </c>
       <c r="B55" t="n">
-        <v>19791200306</v>
+        <v>19781200306</v>
       </c>
       <c r="C55" t="n">
         <v>100</v>
@@ -10132,7 +10133,7 @@
         <v>54</v>
       </c>
       <c r="B56" t="n">
-        <v>20071200307</v>
+        <v>20061200307</v>
       </c>
       <c r="C56" t="n">
         <v>100</v>
@@ -10171,7 +10172,7 @@
         <v>55</v>
       </c>
       <c r="B57" t="n">
-        <v>19871200308</v>
+        <v>19861200308</v>
       </c>
       <c r="C57" t="n">
         <v>100</v>
@@ -10210,7 +10211,7 @@
         <v>56</v>
       </c>
       <c r="B58" t="n">
-        <v>19971200309</v>
+        <v>19961200309</v>
       </c>
       <c r="C58" t="n">
         <v>100</v>
@@ -10249,7 +10250,7 @@
         <v>57</v>
       </c>
       <c r="B59" t="n">
-        <v>19911200310</v>
+        <v>19901200310</v>
       </c>
       <c r="C59" t="n">
         <v>100</v>
@@ -10288,7 +10289,7 @@
         <v>58</v>
       </c>
       <c r="B60" t="n">
-        <v>19791200311</v>
+        <v>19781200311</v>
       </c>
       <c r="C60" t="n">
         <v>90</v>
@@ -10327,7 +10328,7 @@
         <v>59</v>
       </c>
       <c r="B61" t="n">
-        <v>20081200312</v>
+        <v>20071200312</v>
       </c>
       <c r="C61" t="n">
         <v>138</v>
@@ -10366,7 +10367,7 @@
         <v>60</v>
       </c>
       <c r="B62" t="n">
-        <v>20011200313</v>
+        <v>20001200313</v>
       </c>
       <c r="C62" t="n">
         <v>79.5</v>
@@ -10405,7 +10406,7 @@
         <v>61</v>
       </c>
       <c r="B63" t="n">
-        <v>20101200322</v>
+        <v>20091200322</v>
       </c>
       <c r="C63" t="n">
         <v>146</v>
@@ -10444,7 +10445,7 @@
         <v>62</v>
       </c>
       <c r="B64" t="n">
-        <v>19971200335</v>
+        <v>19961200335</v>
       </c>
       <c r="C64" t="n">
         <v>94.7</v>
@@ -10483,7 +10484,7 @@
         <v>63</v>
       </c>
       <c r="B65" t="n">
-        <v>20082100343</v>
+        <v>20072100343</v>
       </c>
       <c r="C65" t="n">
         <v>1961</v>
@@ -10520,7 +10521,7 @@
         <v>64</v>
       </c>
       <c r="B66" t="n">
-        <v>20112100344</v>
+        <v>20102100344</v>
       </c>
       <c r="C66" t="n">
         <v>1961</v>
@@ -10557,7 +10558,7 @@
         <v>65</v>
       </c>
       <c r="B67" t="n">
-        <v>20202100345</v>
+        <v>20192100345</v>
       </c>
       <c r="C67" t="n">
         <v>1961</v>
@@ -10594,7 +10595,7 @@
         <v>66</v>
       </c>
       <c r="B68" t="n">
-        <v>20122100346</v>
+        <v>20112100346</v>
       </c>
       <c r="C68" t="n">
         <v>1961</v>
@@ -10631,7 +10632,7 @@
         <v>67</v>
       </c>
       <c r="B69" t="n">
-        <v>20162100347</v>
+        <v>20152100347</v>
       </c>
       <c r="C69" t="n">
         <v>1961</v>
@@ -10668,7 +10669,7 @@
         <v>68</v>
       </c>
       <c r="B70" t="n">
-        <v>20192100348</v>
+        <v>20182100348</v>
       </c>
       <c r="C70" t="n">
         <v>1961</v>
@@ -10705,7 +10706,7 @@
         <v>69</v>
       </c>
       <c r="B71" t="n">
-        <v>20092100349</v>
+        <v>20082100349</v>
       </c>
       <c r="C71" t="n">
         <v>1961</v>
@@ -10742,7 +10743,7 @@
         <v>70</v>
       </c>
       <c r="B72" t="n">
-        <v>20112100350</v>
+        <v>20102100350</v>
       </c>
       <c r="C72" t="n">
         <v>1961</v>
@@ -10779,7 +10780,7 @@
         <v>71</v>
       </c>
       <c r="B73" t="n">
-        <v>20142100351</v>
+        <v>20132100351</v>
       </c>
       <c r="C73" t="n">
         <v>1961</v>
@@ -10816,7 +10817,7 @@
         <v>72</v>
       </c>
       <c r="B74" t="n">
-        <v>20192100352</v>
+        <v>20182100352</v>
       </c>
       <c r="C74" t="n">
         <v>1961</v>
@@ -10853,7 +10854,7 @@
         <v>73</v>
       </c>
       <c r="B75" t="n">
-        <v>20172100353</v>
+        <v>20162100353</v>
       </c>
       <c r="C75" t="n">
         <v>1961</v>
@@ -10890,7 +10891,7 @@
         <v>74</v>
       </c>
       <c r="B76" t="n">
-        <v>20142100354</v>
+        <v>20132100354</v>
       </c>
       <c r="C76" t="n">
         <v>1961</v>
@@ -10927,7 +10928,7 @@
         <v>75</v>
       </c>
       <c r="B77" t="n">
-        <v>20172100355</v>
+        <v>20162100355</v>
       </c>
       <c r="C77" t="n">
         <v>1961</v>
@@ -10964,7 +10965,7 @@
         <v>76</v>
       </c>
       <c r="B78" t="n">
-        <v>20162100356</v>
+        <v>20152100356</v>
       </c>
       <c r="C78" t="n">
         <v>1961</v>
@@ -11001,7 +11002,7 @@
         <v>77</v>
       </c>
       <c r="B79" t="n">
-        <v>20162100357</v>
+        <v>20152100357</v>
       </c>
       <c r="C79" t="n">
         <v>1961</v>
@@ -11038,7 +11039,7 @@
         <v>78</v>
       </c>
       <c r="B80" t="n">
-        <v>20122100358</v>
+        <v>20112100358</v>
       </c>
       <c r="C80" t="n">
         <v>1961</v>
@@ -11075,7 +11076,7 @@
         <v>79</v>
       </c>
       <c r="B81" t="n">
-        <v>20122100359</v>
+        <v>20112100359</v>
       </c>
       <c r="C81" t="n">
         <v>1961</v>
@@ -11112,7 +11113,7 @@
         <v>80</v>
       </c>
       <c r="B82" t="n">
-        <v>20192100360</v>
+        <v>20182100360</v>
       </c>
       <c r="C82" t="n">
         <v>1961</v>
@@ -11149,7 +11150,7 @@
         <v>81</v>
       </c>
       <c r="B83" t="n">
-        <v>20192100361</v>
+        <v>20182100361</v>
       </c>
       <c r="C83" t="n">
         <v>1961</v>
@@ -11186,7 +11187,7 @@
         <v>82</v>
       </c>
       <c r="B84" t="n">
-        <v>20072100362</v>
+        <v>20062100362</v>
       </c>
       <c r="C84" t="n">
         <v>1961</v>
@@ -11223,7 +11224,7 @@
         <v>83</v>
       </c>
       <c r="B85" t="n">
-        <v>20131200366</v>
+        <v>20121200366</v>
       </c>
       <c r="C85" t="n">
         <v>360</v>
@@ -11262,7 +11263,7 @@
         <v>84</v>
       </c>
       <c r="B86" t="n">
-        <v>20111200377</v>
+        <v>20101200377</v>
       </c>
       <c r="C86" t="n">
         <v>85.3</v>
@@ -11301,7 +11302,7 @@
         <v>85</v>
       </c>
       <c r="B87" t="n">
-        <v>20001200380</v>
+        <v>19991200380</v>
       </c>
       <c r="C87" t="n">
         <v>124</v>
@@ -11340,7 +11341,7 @@
         <v>86</v>
       </c>
       <c r="B88" t="n">
-        <v>19831200381</v>
+        <v>19821200381</v>
       </c>
       <c r="C88" t="n">
         <v>480</v>
@@ -11379,7 +11380,7 @@
         <v>87</v>
       </c>
       <c r="B89" t="n">
-        <v>20031200382</v>
+        <v>20021200382</v>
       </c>
       <c r="C89" t="n">
         <v>143</v>
@@ -11418,7 +11419,7 @@
         <v>88</v>
       </c>
       <c r="B90" t="n">
-        <v>20001200385</v>
+        <v>19991200385</v>
       </c>
       <c r="C90" t="n">
         <v>910</v>
@@ -11457,7 +11458,7 @@
         <v>89</v>
       </c>
       <c r="B91" t="n">
-        <v>20011200393</v>
+        <v>20001200393</v>
       </c>
       <c r="C91" t="n">
         <v>79.7</v>
@@ -11496,7 +11497,7 @@
         <v>90</v>
       </c>
       <c r="B92" t="n">
-        <v>19901200399</v>
+        <v>19891200399</v>
       </c>
       <c r="C92" t="n">
         <v>220</v>
@@ -11847,7 +11848,7 @@
         <v>0</v>
       </c>
       <c r="B2" t="n">
-        <v>20182600079</v>
+        <v>20172600079</v>
       </c>
       <c r="C2" t="inlineStr">
         <is>
@@ -11996,7 +11997,7 @@
           <t>StartTime</t>
         </is>
       </c>
-      <c r="B2" s="7" t="n">
+      <c r="B2" s="8" t="n">
         <v>43830.99861111111</v>
       </c>
     </row>
@@ -12006,7 +12007,7 @@
           <t>StopTime</t>
         </is>
       </c>
-      <c r="B3" s="7" t="n">
+      <c r="B3" s="8" t="n">
         <v>44195.99861111111</v>
       </c>
     </row>

</xml_diff>